<commit_message>
Moved to week 4
</commit_message>
<xml_diff>
--- a/result_list.xlsx
+++ b/result_list.xlsx
@@ -458,12 +458,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Boston Beer Bellies (3)</t>
+          <t>Boston Beer Bellies (6)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Team Becks (7)</t>
+          <t>Team Blah (4)</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -471,59 +471,59 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Team Becks</t>
+          <t>Boston Beer Bellies</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Brunson Burner (4)</t>
+          <t>Brunson Burner (6)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Mo' Money Mo Bamba (7)</t>
+          <t>Mos Eisley Banthas (4)</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Mo' Money Mo Bamba</t>
+          <t>Brunson Burner</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Gaza Gunners (7)</t>
+          <t>Giddey Up Chumps (5)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jazz (3)</t>
+          <t>Jazzy J (3)</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Gaza Gunners</t>
+          <t>Giddey Up Chumps</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Flint Tropics (4)</t>
+          <t>Fox Force 5 (3)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Los Angeles Ballerz (6)</t>
+          <t>Luka Deez Nuts (7)</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -531,99 +531,99 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Los Angeles Ballerz</t>
+          <t>Luka Deez Nuts</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>GIDDEY UPS (7)</t>
+          <t>Gladysisahoe Dazz (3)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>The IBINATORS (4)</t>
+          <t>The Mighty Bears (6)</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>GIDDEY UPS</t>
+          <t>The Mighty Bears</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Chi Cargo Pants (7)</t>
+          <t>Chi Cargo Pants (5)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>KING JAMIS (2)</t>
+          <t>KJ's DM's (6)</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Chi Cargo Pants</t>
+          <t>KJ's DM's</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Champ is here (3)</t>
+          <t>Champ is here (4)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Harrison the league (8)</t>
+          <t>Helltown Hops (6)</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Harrison the league</t>
+          <t>Helltown Hops</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Logan Bogans (5)</t>
+          <t>Lucky Punters (7)</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Memphis 12 Guage (6)</t>
+          <t>Miami Heat Checks (3)</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Memphis 12 Guage</t>
+          <t>Lucky Punters</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>FrostyFlyers (1)</t>
+          <t>Funghi Curry (4)</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Giddey Up Chumps (9)</t>
+          <t>GIDDEY UPS (6)</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -631,14 +631,14 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Giddey Up Chumps</t>
+          <t>GIDDEY UPS</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Desmond’s Dynasty (4)</t>
+          <t>Desmond’s Dynasty (3)</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -647,7 +647,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -658,72 +658,72 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>On The Bagleys (4)</t>
+          <t>Pablo's Players (3)</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Team Wallace (6)</t>
+          <t>Team Winchester (6)</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Team Wallace</t>
+          <t>Team Winchester</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Average Joes (5)</t>
+          <t>Average Joes (6)</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Phoenix Gray Hammers (6)</t>
+          <t>Please Hammer don't Huerter (4)</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Phoenix Gray Hammers</t>
+          <t>Average Joes</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Brooklyn 99 (6)</t>
+          <t>Brooklyn 99 (3)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Mos Eisley Banthas (5)</t>
+          <t>Moves Like Agger (7)</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Brooklyn 99</t>
+          <t>Moves Like Agger</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Brooks, Crooks and Sooks (6)</t>
+          <t>Brooks, Crooks and Sooks (7)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Karl Anthony's CLOWNS (4)</t>
+          <t>KING JAMIS (3)</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -738,32 +738,32 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>$picy ball (5)</t>
+          <t>'22 Spirit (6)</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Landsdale Smith (6)</t>
+          <t>Lick DeBallZachs (4)</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Landsdale Smith</t>
+          <t>'22 Spirit</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Keyonte George Costanza (6)</t>
+          <t>Kingcalvin (4)</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Team No Lackin (4)</t>
+          <t>Team Pyke (6)</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -771,39 +771,39 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Keyonte George Costanza</t>
+          <t>Team Pyke</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Philderbeasts (3)</t>
+          <t>pingu123 (3)</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Under my Clint Capela (7)</t>
+          <t>Victor Oladeepthr*ats (6)</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Under my Clint Capela</t>
+          <t>Victor Oladeepthr*ats</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Splash Bros 3011 (4)</t>
+          <t>Sweet Home Wembanyama (6)</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Who what where when Kawhi (6)</t>
+          <t>Who what where when Kawhi (4)</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -811,19 +811,19 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Who what where when Kawhi</t>
+          <t>Sweet Home Wembanyama</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Beau_Brigade (3)</t>
+          <t>Beau_Brigade (5)</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>The David Cahill's (7)</t>
+          <t>The Flaming Galahs (6)</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -831,39 +831,39 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>The David Cahill's</t>
+          <t>The Flaming Galahs</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Ol' Dirty Baskets (8)</t>
+          <t>OnlyFranz (5)</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Revenge of The Cedi (3)</t>
+          <t>Rikroller (6)</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Ol' Dirty Baskets</t>
+          <t>Rikroller</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Dallas Double D's (7)</t>
+          <t>Dallas Double D's (4)</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Jackie Daytona (3)</t>
+          <t>James and the Giant Overreach (6)</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -871,19 +871,19 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Dallas Double D's</t>
+          <t>James and the Giant Overreach</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Funghi Curry (6)</t>
+          <t>G-Town DownTowners (7)</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Its on like Doncic Kong (4)</t>
+          <t>It’s the Final KAT-Towns (3)</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -891,19 +891,19 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Funghi Curry</t>
+          <t>G-Town DownTowners</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Frank Reynolds (4)</t>
+          <t>Fresh Prince FP (3)</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>TankCity Unicorns (6)</t>
+          <t>Team Alcobio (7)</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -911,47 +911,47 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>TankCity Unicorns</t>
+          <t>Team Alcobio</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Matisse Fly Bulls (7)</t>
+          <t>Memphis 12 Guage (2)</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>New Orleans Zionlyfans (2)</t>
+          <t>North Noosa Leather Jackets (9)</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Matisse Fly Bulls</t>
+          <t>North Noosa Leather Jackets</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>JR Swishes (2)</t>
+          <t>Keyonte George Costanza (2)</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>VICTOR-IOUS (9)</t>
+          <t>Wandering Bears (8)</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>VICTOR-IOUS</t>
+          <t>Wandering Bears</t>
         </is>
       </c>
     </row>
@@ -963,7 +963,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>OKC-OOPS (8)</t>
+          <t>On The Bagleys (8)</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -971,19 +971,19 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>OKC-OOPS</t>
+          <t>On The Bagleys</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>ESU (2)</t>
+          <t>ESU (6)</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Tennant Creek Big Horses (8)</t>
+          <t>The A**L Embiids (4)</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -991,39 +991,39 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Tennant Creek Big Horses</t>
+          <t>ESU</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Team irwin (7)</t>
+          <t>Team James (7)</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Team Winchester (3)</t>
+          <t>Team Z3LLY (2)</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Team irwin</t>
+          <t>Team James</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Asian Zing (0)</t>
+          <t>Asian Zing (6)</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Edward St Easybeats (10)</t>
+          <t>Edward St Easybeats (4)</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -1031,19 +1031,19 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Edward St Easybeats</t>
+          <t>Asian Zing</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>In Touch With The Common Man (4)</t>
+          <t>Indiana Monstars (7)</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Victor WembanYoMama (6)</t>
+          <t>VICTOR-IOUS (3)</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -1051,19 +1051,19 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Victor WembanYoMama</t>
+          <t>Indiana Monstars</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Flex n Affect (6)</t>
+          <t>Flint Michigan tropics (2)</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Jinja Go Bear (4)</t>
+          <t>Joe Hablo Ingles (8)</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -1071,19 +1071,19 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Flex n Affect</t>
+          <t>Joe Hablo Ingles</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Moon Shooters (7)</t>
+          <t>Motor Cade (4)</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>WORST EVER (3)</t>
+          <t>WORST EVER (6)</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -1091,19 +1091,19 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Moon Shooters</t>
+          <t>WORST EVER</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>pingu123 (1)</t>
+          <t>Plumlees Crack (9)</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>The Plasticman (9)</t>
+          <t>The Sengunies (1)</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -1111,19 +1111,19 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>The Plasticman</t>
+          <t>Plumlees Crack</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Jimmy Brings (6)</t>
+          <t>Jimmy ButtPlugs (6)</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Joe Mamma's drama llamas (4)</t>
+          <t>JR Swishes (5)</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -1131,19 +1131,19 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Jimmy Brings</t>
+          <t>Jimmy ButtPlugs</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Slovenia. Beer. Dallas (7)</t>
+          <t>Splash Bros 3011 (4)</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Wandering Bears (3)</t>
+          <t>War Grimes in Garza (6)</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -1151,19 +1151,19 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Slovenia. Beer. Dallas</t>
+          <t>War Grimes in Garza</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Daryl's Discount Dimes (8)</t>
+          <t>Daryl's Discount Dimes (6)</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Kobe Wan Kenobi (2)</t>
+          <t>LA Anthony Day-to-Davis (5)</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -1178,12 +1178,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Minnesota Lumberjacks (7)</t>
+          <t>Mo' Money Mo Bamba (0)</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Yippie Kyrie Motherf**ker (3)</t>
+          <t>Yippie Kyrie Motherf**ker (10)</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1191,23 +1191,23 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Minnesota Lumberjacks</t>
+          <t>Yippie Kyrie Motherf**ker</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Adelaide Shed Shots (4)</t>
+          <t>Adelaide Shed Shots (7)</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>HotDawgs (3)</t>
+          <t>Houston Mob Squad (3)</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1218,12 +1218,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Embiid's Flavour Town (3)</t>
+          <t>Embiid's Flavour Town (6)</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>New York NateThrobinsons (7)</t>
+          <t>nutted In her Gasol (4)</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>New York NateThrobinsons</t>
+          <t>Embiid's Flavour Town</t>
         </is>
       </c>
     </row>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Doris' Big Old Giddies (4)</t>
+          <t>Doris' Big Old Giddies (5)</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -1258,12 +1258,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>MrPenPen (4)</t>
+          <t>My team sucks. Damn. (4)</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Team Blah (6)</t>
+          <t>Team Cooke (6)</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -1271,103 +1271,103 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Team Blah</t>
+          <t>Team Cooke</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Bruce brown-eye (4)</t>
+          <t>Bruce brown-eye (3)</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>The Chet Code (6)</t>
+          <t>The David Cahill's (6)</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>The Chet Code</t>
+          <t>The David Cahill's</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Luka Warm (7)</t>
+          <t>Margaret River Wyld Stallyns (8)</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>nutted In her Gasol (4)</t>
+          <t>OG Wan Unobi (2)</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Luka Warm</t>
+          <t>Margaret River Wyld Stallyns</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>HARDEN UP! (4)</t>
+          <t>Harrison the league (7)</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Team Cumming (5)</t>
+          <t>Team Damon (3)</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Team Cumming</t>
+          <t>Harrison the league</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Team James (6)</t>
+          <t>Team luka slo (5)</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Team Z3LLY (4)</t>
+          <t>Temporary Linsanity (4)</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Team James</t>
+          <t>Team luka slo</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Balls Deep (5)</t>
+          <t>Balls Deep (7)</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>DominAyton Curry (4)</t>
+          <t>DominAyton Curry (3)</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -1378,36 +1378,36 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Lewisham Loose Units (4)</t>
+          <t>Lil Bow Yaus (6)</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Scottie Pippings (5)</t>
+          <t>Seattle SuperChronics (5)</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Scottie Pippings</t>
+          <t>Lil Bow Yaus</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Browntown (6)</t>
+          <t>Browntown (7)</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>OG Tassie Devils (5)</t>
+          <t>OKC-OOPS (2)</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -1418,32 +1418,32 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>DurdyDurdsDuds (2)</t>
+          <t>DurdyDurdsDuds (6)</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Lucky Punters (9)</t>
+          <t>Luka Warm (5)</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Lucky Punters</t>
+          <t>DurdyDurdsDuds</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Gladysisahoe Dazz (6)</t>
+          <t>Globetrotter Gunts (6)</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Sleepers (4)</t>
+          <t>Slim Towers (4)</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1451,19 +1451,19 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Gladysisahoe Dazz</t>
+          <t>Globetrotter Gunts</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Lil Bow Yaus (3)</t>
+          <t>Little Buff Boys (2)</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Team Thomas (6)</t>
+          <t>Team Wallace (7)</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1471,34 +1471,34 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Team Thomas</t>
+          <t>Team Wallace</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Bronsexual Lebrolites (8)</t>
+          <t>Bronsexual Lebrolites (3)</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Slim Towers (3)</t>
+          <t>Slovenia. Beer. Dallas (6)</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Bronsexual Lebrolites</t>
+          <t>Slovenia. Beer. Dallas</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Atlanta Waivers (7)</t>
+          <t>Atlanta Waivers (6)</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1507,7 +1507,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -1518,52 +1518,52 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Insert Team Name Here (6)</t>
+          <t>It's Always F'd In Philadelphia (6)</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Team Nicholson (4)</t>
+          <t>Team No Lackin (3)</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Insert Team Name Here</t>
+          <t>It's Always F'd In Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Greek Freaks (2)</t>
+          <t>H I (2)</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Taiwan Troopers (9)</t>
+          <t>TankCity Unicorns (7)</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Taiwan Troopers</t>
+          <t>TankCity Unicorns</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Fantasyland Basketball Podcast (8)</t>
+          <t>FIGJAM (7)</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>North Noosa Leather Jackets (2)</t>
+          <t>OG Tassie Devils (3)</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -1571,7 +1571,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Fantasyland Basketball Podcast</t>
+          <t>FIGJAM</t>
         </is>
       </c>
     </row>
@@ -1583,11 +1583,11 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Rodney Rodgers (4)</t>
+          <t>ROUdiamondGH (3)</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -1598,52 +1598,52 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Jaylen CAN go left! (6)</t>
+          <t>Jazz (7)</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Pablo's Players (5)</t>
+          <t>Peeattle Poopersonics (2)</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Jaylen CAN go left!</t>
+          <t>Jazz</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>50 Shades of Shai (3)</t>
+          <t>50 Shades of Shai (7)</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Mile High Mutombo's (7)</t>
+          <t>misq (2)</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Mile High Mutombo's</t>
+          <t>50 Shades of Shai</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Boswell Pioneers (7)</t>
+          <t>Boswell Pioneers (8)</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Taco Corp (3)</t>
+          <t>Taiwan Troopers (2)</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -1658,12 +1658,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Hispanic Deepers (6)</t>
+          <t>Holy Klay-Noli's (4)</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Meep Meep (4)</t>
+          <t>Miami Butlers (6)</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -1671,19 +1671,19 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Hispanic Deepers</t>
+          <t>Miami Butlers</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Arizoey Magic (3)</t>
+          <t>Arizoey Magic (2)</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Boots Manuva (7)</t>
+          <t>Boots Manuva (8)</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -1698,32 +1698,32 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Miami Heat Checks (7)</t>
+          <t>Minnesota Lumberjacks (4)</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Sideline Out of Bounds (4)</t>
+          <t>Signature Moves (6)</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Miami Heat Checks</t>
+          <t>Signature Moves</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Little Buff Boys (8)</t>
+          <t>Logan Bogans (6)</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Seattle Superchronics (2)</t>
+          <t>Shanghai Sharks (4)</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -1731,59 +1731,59 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Little Buff Boys</t>
+          <t>Logan Bogans</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>LaMarc Gasoldridge (1)</t>
+          <t>Lewisham Loose Units (8)</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>LIL UZI YURT (9)</t>
+          <t>Livin' La Vida Luka (3)</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>LIL UZI YURT</t>
+          <t>Lewisham Loose Units</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Donnys Beans (7)</t>
+          <t>Donnys Beans (4)</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Mr. 4th Quarter (4)</t>
+          <t>Murphys Misfits (6)</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Donnys Beans</t>
+          <t>Murphys Misfits</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>GOLD COAST GREMLINS (8)</t>
+          <t>Good Problems (8)</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Team Mercer (2)</t>
+          <t>Team Nicholson (2)</t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -1791,19 +1791,19 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>GOLD COAST GREMLINS</t>
+          <t>Good Problems</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>AY JARAMBA! (4)</t>
+          <t>AY JARAMBA! (5)</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Quit Javing me turky (6)</t>
+          <t>Rated PG13 (6)</t>
         </is>
       </c>
       <c r="C69" t="n">
@@ -1811,19 +1811,19 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Quit Javing me turky</t>
+          <t>Rated PG13</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Couch potatoes (4)</t>
+          <t>Couch potatoes (2)</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Globetrotter Gunts (6)</t>
+          <t>GOLD COAST GREMLINS (8)</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -1831,19 +1831,19 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Globetrotter Gunts</t>
+          <t>GOLD COAST GREMLINS</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>'22 Spirit (6)</t>
+          <t>$picy ball (6)</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>It's Always F'd In Philadelphia (5)</t>
+          <t>Its on like Doncic Kong (4)</t>
         </is>
       </c>
       <c r="C71" t="n">
@@ -1851,23 +1851,23 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>'22 Spirit</t>
+          <t>$picy ball</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Bames Jond (7)</t>
+          <t>Bames Jond (8)</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Rikroller (3)</t>
+          <t>Rodney Rodgers (3)</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -1883,7 +1883,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Jimmy ButtPlugs (5)</t>
+          <t>Jinja Go Bear (4)</t>
         </is>
       </c>
       <c r="C73" t="n">
@@ -1898,12 +1898,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>G-Town DownTowners (3)</t>
+          <t>Gaza Gunners (7)</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Team Hewish (7)</t>
+          <t>Team irwin (3)</t>
         </is>
       </c>
       <c r="C74" t="n">
@@ -1911,34 +1911,34 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Team Hewish</t>
+          <t>Gaza Gunners</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>BigZ Spurs (8)</t>
+          <t>BigZ Spurs (4)</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Down Right Sneaky (3)</t>
+          <t>Down Right Sneaky (5)</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>BigZ Spurs</t>
+          <t>Down Right Sneaky</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Bair Jordan (3)</t>
+          <t>Bair Jordan (4)</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -1947,7 +1947,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -1958,20 +1958,20 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>DY PJ Birch (5)</t>
+          <t>DY PJ Birch (4)</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Triple Towers (6)</t>
+          <t>Uncle Ben (4)</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Triple Towers</t>
+          <t>Darwin Esky</t>
         </is>
       </c>
     </row>
@@ -1983,47 +1983,47 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>The Blue Mountain Goats (8)</t>
+          <t>The Book of Irving (7)</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>The Blue Mountain Goats</t>
+          <t>The Book of Irving</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Moves Like Agger (6)</t>
+          <t>MrPenPen (9)</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Team Alcobio (5)</t>
+          <t>Team Ashton (2)</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Moves Like Agger</t>
+          <t>MrPenPen</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Ben Simmons For 3 (4)</t>
+          <t>Ben Simmons For 3 (3)</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Zions Illegitimate Child (6)</t>
+          <t>Zions Illegitimate Child (7)</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -2038,12 +2038,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>I Felton Her Booby (5)</t>
+          <t>In Touch With The Common Man (2)</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>SavedByTheKelle (6)</t>
+          <t>Scottie Pippings (8)</t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -2051,19 +2051,19 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>SavedByTheKelle</t>
+          <t>Scottie Pippings</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>It’s the Final KAT-Towns (2)</t>
+          <t>Ja 'his real name is Clarence' (3)</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>LA Anthony Day-to-Davis (8)</t>
+          <t>Landsdale Smith (7)</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -2071,59 +2071,59 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>LA Anthony Day-to-Davis</t>
+          <t>Landsdale Smith</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Miami Butlers (3)</t>
+          <t>Mile High Mutombo's (3)</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>The Great Hali (7)</t>
+          <t>The Hairy Skips (6)</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>The Great Hali</t>
+          <t>The Hairy Skips</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Aussie Goats (5)</t>
+          <t>Aussie Goats (8)</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Victor Oladeepthr*ats (6)</t>
+          <t>Victor WembanYoMama (3)</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Victor Oladeepthr*ats</t>
+          <t>Aussie Goats</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>ROUdiamondGH (7)</t>
+          <t>Round Mound of Rebound (2)</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>The Sengunies (3)</t>
+          <t>The Shrimp Nets (8)</t>
         </is>
       </c>
       <c r="C85" t="n">
@@ -2131,39 +2131,39 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>ROUdiamondGH</t>
+          <t>The Shrimp Nets</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Holy Klay-Noli's (4)</t>
+          <t>HotDawgs (1)</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Margaret River Wyld Stallyns (7)</t>
+          <t>Meep Meep (9)</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Margaret River Wyld Stallyns</t>
+          <t>Meep Meep</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>KJ's DM's (5)</t>
+          <t>Kobe Beans (3)</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>OG Wan Unobi (6)</t>
+          <t>Ol' Dirty Baskets (7)</t>
         </is>
       </c>
       <c r="C87" t="n">
@@ -2171,19 +2171,19 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>OG Wan Unobi</t>
+          <t>Ol' Dirty Baskets</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Team Damon (6)</t>
+          <t>Team Hewish (3)</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>The Mighty Bears (4)</t>
+          <t>The Plasticman (7)</t>
         </is>
       </c>
       <c r="C88" t="n">
@@ -2191,39 +2191,39 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Team Damon</t>
+          <t>The Plasticman</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Bulls (8)</t>
+          <t>Bulls (3)</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Livin' La Vida Luka (3)</t>
+          <t>Los Angeles Ballerz (7)</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Bulls</t>
+          <t>Los Angeles Ballerz</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Bank Town Squids (7)</t>
+          <t>Bank Town Squids (6)</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Wizbangs' Warriors (3)</t>
+          <t>Wizbangs' Warriors (4)</t>
         </is>
       </c>
       <c r="C90" t="n">
@@ -2238,12 +2238,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>The Wrath (3)</t>
+          <t>Townsville Crocs (5)</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>You Don't Mess with the Ant-Man (7)</t>
+          <t>You Don't Mess with the Ant-Man (6)</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -2258,12 +2258,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>T-I-M….Team!! (4)</t>
+          <t>Taco Corp (8)</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Uncle Ben (6)</t>
+          <t>Under my Clint Capela (2)</t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -2271,47 +2271,47 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Uncle Ben</t>
+          <t>Taco Corp</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Bird Sprog (3)</t>
+          <t>Bird Sprog (6)</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>The Hairy Skips (8)</t>
+          <t>The IBINATORS (5)</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>The Hairy Skips</t>
+          <t>Bird Sprog</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>OnlyFranz (5)</t>
+          <t>Panania Rockets (2)</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Sweet Home Wembanyama (3)</t>
+          <t>T-I-M….Team!! (8)</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>OnlyFranz</t>
+          <t>T-I-M….Team!!</t>
         </is>
       </c>
     </row>
@@ -2323,7 +2323,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>The Shrimp Nets (4)</t>
+          <t>The Wrath (4)</t>
         </is>
       </c>
       <c r="C95" t="n">
@@ -2338,32 +2338,32 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>The Bricks (4)</t>
+          <t>The Chet Code (6)</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Weekend at Boogie's (6)</t>
+          <t>Weekend at Boogie's (5)</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Weekend at Boogie's</t>
+          <t>The Chet Code</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Helltown Hops (2)</t>
+          <t>Hispanic Deepers (6)</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>The Book of Irving (8)</t>
+          <t>The Bricks (4)</t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -2371,59 +2371,59 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>The Book of Irving</t>
+          <t>Hispanic Deepers</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Saint Lunatics (3)</t>
+          <t>SavedByTheKelle (4)</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>THE FRESH PRINCE OF GC (8)</t>
+          <t>The Gee Whizzles (6)</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>THE FRESH PRINCE OF GC</t>
+          <t>The Gee Whizzles</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Seattle SuperChronics (7)</t>
+          <t>Seattle Superchronics (2)</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Team Rah to the Max (4)</t>
+          <t>Team Thomas (8)</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Seattle SuperChronics</t>
+          <t>Team Thomas</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Brisbane Noble’s Nobs (6)</t>
+          <t>Brisbane Noble’s Nobs (7)</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>punting everything (4)</t>
+          <t>Quit Javing me turky (3)</t>
         </is>
       </c>
       <c r="C100" t="n">
@@ -2438,52 +2438,52 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>My team sucks. Damn. (1)</t>
+          <t>New York NateThrobinsons (1)</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Panania Rockets (9)</t>
+          <t>Philderbeasts (8)</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Panania Rockets</t>
+          <t>Philderbeasts</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Ja 'his real name is Clarence' (9)</t>
+          <t>Ja Raffe (5)</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>The Gee Whizzles (1)</t>
+          <t>The Great Hali (4)</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Ja 'his real name is Clarence'</t>
+          <t>Ja Raffe</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Cossi's Carnts (4)</t>
+          <t>Cossi's Carnts (6)</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Team luka slo (6)</t>
+          <t>Team Mercer (4)</t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -2491,39 +2491,39 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Team luka slo</t>
+          <t>Cossi's Carnts</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Canada Demon (4)</t>
+          <t>Canada Demon (5)</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Caruso BaldEagles (6)</t>
+          <t>Caruso BaldEagles (4)</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Caruso BaldEagles</t>
+          <t>Canada Demon</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Houston Mob Squad (7)</t>
+          <t>I Felton Her Booby (5)</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Murphys Misfits (3)</t>
+          <t>New Orleans Zionlyfans (6)</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -2531,19 +2531,19 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Houston Mob Squad</t>
+          <t>New Orleans Zionlyfans</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Good Problems (3)</t>
+          <t>Greek Freaks (7)</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Townsville Crocs (7)</t>
+          <t>Triple Towers (3)</t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -2551,19 +2551,19 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Townsville Crocs</t>
+          <t>Greek Freaks</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Big Bam Theory (6)</t>
+          <t>Big Bam Theory (7)</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Motor Cade (4)</t>
+          <t>Mr. 4th Quarter (3)</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -2578,32 +2578,32 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Indiana Monstars (8)</t>
+          <t>Insert Team Name Here (3)</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Lick DeBallZachs (3)</t>
+          <t>LIL UZI YURT (6)</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Indiana Monstars</t>
+          <t>LIL UZI YURT</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Ben Simmons Construction (6)</t>
+          <t>Ben Simmons Construction (3)</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Jazzy J (5)</t>
+          <t>Jimmy Brings (7)</t>
         </is>
       </c>
       <c r="C109" t="n">
@@ -2611,19 +2611,19 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Ben Simmons Construction</t>
+          <t>Jimmy Brings</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Knock the Toppin off (3)</t>
+          <t>Kobe Wan Kenobi (9)</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Red Dragons (7)</t>
+          <t>Revenge of The Cedi (1)</t>
         </is>
       </c>
       <c r="C110" t="n">
@@ -2631,39 +2631,39 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Red Dragons</t>
+          <t>Kobe Wan Kenobi</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Fresh Prince FP (4)</t>
+          <t>FrostyFlyers (6)</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Joeys Mad Lads (7)</t>
+          <t>Karl Anthony's CLOWNS (5)</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Joeys Mad Lads</t>
+          <t>FrostyFlyers</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Kingcalvin (8)</t>
+          <t>Knock the Toppin off (7)</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Preying Domantas (2)</t>
+          <t>punting everything (3)</t>
         </is>
       </c>
       <c r="C112" t="n">
@@ -2671,39 +2671,39 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Kingcalvin</t>
+          <t>Knock the Toppin off</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Fox Force 5 (3)</t>
+          <t>Frank Reynolds (1)</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Luka Deez Nuts (6)</t>
+          <t>Mamba Mentality (9)</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Luka Deez Nuts</t>
+          <t>Mamba Mentality</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Mamba Mentality (3)</t>
+          <t>Matisse Fly Bulls (3)</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Team Pyke (7)</t>
+          <t>Team Rah to the Max (7)</t>
         </is>
       </c>
       <c r="C114" t="n">
@@ -2711,39 +2711,39 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Team Pyke</t>
+          <t>Team Rah to the Max</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Signature Moves (9)</t>
+          <t>Sleepers (3)</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Temporary Linsanity (2)</t>
+          <t>Tennant Creek Big Horses (7)</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Signature Moves</t>
+          <t>Tennant Creek Big Horses</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Ja Raffe (7)</t>
+          <t>Jackie Daytona (6)</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Shwin's Ballsdeep (3)</t>
+          <t>Sideline Out of Bounds (5)</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -2751,19 +2751,19 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Ja Raffe</t>
+          <t>Jackie Daytona</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>All the Ingles ladies (5)</t>
+          <t>All the Ingles ladies (1)</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Joe Hablo Ingles (6)</t>
+          <t>Joeys Mad Lads (9)</t>
         </is>
       </c>
       <c r="C117" t="n">
@@ -2771,19 +2771,19 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Joe Hablo Ingles</t>
+          <t>Joeys Mad Lads</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>FIGJAM (4)</t>
+          <t>Flex n Affect (7)</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Kobe Beans (6)</t>
+          <t>Kripsy Strips Porzingerbox (3)</t>
         </is>
       </c>
       <c r="C118" t="n">
@@ -2791,39 +2791,39 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Kobe Beans</t>
+          <t>Flex n Affect</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>The A**L Embiids (2)</t>
+          <t>The Blue Mountain Goats (6)</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>The Flaming Galahs (9)</t>
+          <t>THE FRESH PRINCE OF GC (3)</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>The Flaming Galahs</t>
+          <t>The Blue Mountain Goats</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Dort Stop Believin (7)</t>
+          <t>Dort Stop Believin (10)</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Rated PG13 (3)</t>
+          <t>Re dirkulous (0)</t>
         </is>
       </c>
       <c r="C120" t="n">
@@ -2838,12 +2838,12 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Flint Michigan tropics (4)</t>
+          <t>Flint Tropics (8)</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Round Mound of Rebound (6)</t>
+          <t>Saint Lunatics (2)</t>
         </is>
       </c>
       <c r="C121" t="n">
@@ -2851,19 +2851,19 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Round Mound of Rebound</t>
+          <t>Flint Tropics</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Hard Solo (8)</t>
+          <t>HARDEN UP! (7)</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Kripsy Strips Porzingerbox (2)</t>
+          <t>LaMarc Gasoldridge (3)</t>
         </is>
       </c>
       <c r="C122" t="n">
@@ -2871,39 +2871,39 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Hard Solo</t>
+          <t>HARDEN UP!</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>misq (9)</t>
+          <t>Moon Shooters (7)</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Team Ashton (1)</t>
+          <t>Team Becks (2)</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>misq</t>
+          <t>Moon Shooters</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Boston Bombers (8)</t>
+          <t>Boston Bombers (6)</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Re dirkulous (2)</t>
+          <t>Red Dragons (4)</t>
         </is>
       </c>
       <c r="C124" t="n">
@@ -2918,27 +2918,27 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Allen Iversons Ego (5)</t>
+          <t>Allen Iversons Ego (8)</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Don't Go Blakin My Heart (6)</t>
+          <t>Don't Go Blakin My Heart (2)</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Don't Go Blakin My Heart</t>
+          <t>Allen Iversons Ego</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Boomtown Bulls (6)</t>
+          <t>Boomtown Bulls (5)</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -2947,7 +2947,7 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D126" t="inlineStr">
         <is>
@@ -2958,52 +2958,52 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Shanghai Sharks (6)</t>
+          <t>Shwin's Ballsdeep (6)</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Wembanyama but 5'10 (3)</t>
+          <t>Wembanyama but 5'10 (4)</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Shanghai Sharks</t>
+          <t>Shwin's Ballsdeep</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Boston Ballerz (7)</t>
+          <t>Boston Ballerz (1)</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>H I (4)</t>
+          <t>Hard Solo (9)</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Boston Ballerz</t>
+          <t>Hard Solo</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Duncans Donuts (7)</t>
+          <t>Duncans Donuts (6)</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Team Cooke (3)</t>
+          <t>Team Cumming (4)</t>
         </is>
       </c>
       <c r="C129" t="n">
@@ -3018,32 +3018,32 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Bench Boys (2)</t>
+          <t>Bench Boys (7)</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>James and the Giant Overreach (7)</t>
+          <t>Jaylen CAN go left! (3)</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>James and the Giant Overreach</t>
+          <t>Bench Boys</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Peeattle Poopersonics (8)</t>
+          <t>Phoenix Gray Hammers (4)</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Plumlees Crack (2)</t>
+          <t>Preying Domantas (6)</t>
         </is>
       </c>
       <c r="C131" t="n">
@@ -3051,7 +3051,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Peeattle Poopersonics</t>
+          <t>Preying Domantas</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added league info to schedule
</commit_message>
<xml_diff>
--- a/result_list.xlsx
+++ b/result_list.xlsx
@@ -458,12 +458,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Mos Eisley Banthas (6)</t>
+          <t>Mos Eisley Banthas (7)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Team Blah (5)</t>
+          <t>Team Blah (4)</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -558,12 +558,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Please Hammer don't Huerter (6)</t>
+          <t>Please Hammer don't Huerter (3)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Team Winchester (3)</t>
+          <t>Team Winchester (6)</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -571,7 +571,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Please Hammer don't Huerter</t>
+          <t>Team Winchester</t>
         </is>
       </c>
     </row>
@@ -718,12 +718,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Team James (4)</t>
+          <t>Team James (3)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>The A**L Embiids (6)</t>
+          <t>The A**L Embiids (7)</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -738,12 +738,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Edward St Easybeats (6)</t>
+          <t>Edward St Easybeats (4)</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>VICTOR-IOUS (4)</t>
+          <t>VICTOR-IOUS (6)</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -751,7 +751,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Edward St Easybeats</t>
+          <t>VICTOR-IOUS</t>
         </is>
       </c>
     </row>
@@ -858,20 +858,20 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Team Cooke (4)</t>
+          <t>Team Cooke (6)</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>The David Cahill's (5)</t>
+          <t>The David Cahill's (4)</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>The David Cahill's</t>
+          <t>Team Cooke</t>
         </is>
       </c>
     </row>
@@ -898,12 +898,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Balls Deep (6)</t>
+          <t>Balls Deep (7)</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Team luka slo (4)</t>
+          <t>Team luka slo (3)</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -918,7 +918,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Browntown (4)</t>
+          <t>Browntown (3)</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -927,7 +927,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1038,12 +1038,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Boswell Pioneers (8)</t>
+          <t>Boswell Pioneers (7)</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>misq (2)</t>
+          <t>misq (3)</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -1238,16 +1238,16 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Scottie Pippings (6)</t>
+          <t>Scottie Pippings (5)</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Zions Illegitimate Child (2)</t>
+          <t>Zions Illegitimate Child (4)</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1298,16 +1298,16 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Meep Meep (8)</t>
+          <t>Meep Meep (6)</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Ol' Dirty Baskets (2)</t>
+          <t>Ol' Dirty Baskets (5)</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -1318,12 +1318,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Bulls (8)</t>
+          <t>Bulls (6)</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Team Hewish (3)</t>
+          <t>Team Hewish (5)</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1338,12 +1338,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Bank Town Squids (4)</t>
+          <t>Bank Town Squids (6)</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>You Don't Mess with the Ant-Man (6)</t>
+          <t>You Don't Mess with the Ant-Man (4)</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1351,7 +1351,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>You Don't Mess with the Ant-Man</t>
+          <t>Bank Town Squids</t>
         </is>
       </c>
     </row>
@@ -1438,7 +1438,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Brisbane Noble’s Nobs (3)</t>
+          <t>Brisbane Noble’s Nobs (4)</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1447,7 +1447,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -1458,12 +1458,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Ja Raffe (6)</t>
+          <t>Ja Raffe (7)</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Team Mercer (4)</t>
+          <t>Team Mercer (3)</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1498,16 +1498,16 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Big Bam Theory (3)</t>
+          <t>Big Bam Theory (5)</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Triple Towers (7)</t>
+          <t>Triple Towers (6)</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -1663,11 +1663,11 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Moon Shooters (6)</t>
+          <t>Moon Shooters (5)</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -1698,12 +1698,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Boomtown Bulls (6)</t>
+          <t>Boomtown Bulls (4)</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Shanghai Sharks (5)</t>
+          <t>Shanghai Sharks (6)</t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -1711,19 +1711,19 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Boomtown Bulls</t>
+          <t>Shanghai Sharks</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Boston Ballerz (2)</t>
+          <t>Boston Ballerz (3)</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Duncans Donuts (8)</t>
+          <t>Duncans Donuts (7)</t>
         </is>
       </c>
       <c r="C65" t="n">

</xml_diff>

<commit_message>
Updated for week 5
</commit_message>
<xml_diff>
--- a/result_list.xlsx
+++ b/result_list.xlsx
@@ -458,560 +458,560 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Mos Eisley Banthas (7)</t>
+          <t>Mos Eisley Banthas (0)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Team Blah (4)</t>
+          <t>Team Blah (0)</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Mos Eisley Banthas</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Giddey Up Chumps (6)</t>
+          <t>Giddey Up Chumps (0)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Luka Deez Nuts (5)</t>
+          <t>Luka Deez Nuts (0)</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Giddey Up Chumps</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Chi Cargo Pants (6)</t>
+          <t>Chi Cargo Pants (0)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Gladysisahoe Dazz (5)</t>
+          <t>Gladysisahoe Dazz (0)</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Chi Cargo Pants</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Helltown Hops (8)</t>
+          <t>Helltown Hops (0)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Miami Heat Checks (2)</t>
+          <t>Miami Heat Checks (0)</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Helltown Hops</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>GIDDEY UPS (4)</t>
+          <t>GIDDEY UPS (0)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Wham Bam Thankyou Ma’am (5)</t>
+          <t>Wham Bam Thankyou Ma’am (0)</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Wham Bam Thankyou Ma’am</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Please Hammer don't Huerter (3)</t>
+          <t>Please Hammer don't Huerter (0)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Team Winchester (6)</t>
+          <t>Team Winchester (0)</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Team Winchester</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Brooklyn 99 (2)</t>
+          <t>Brooklyn 99 (0)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Brooks, Crooks and Sooks (7)</t>
+          <t>Brooks, Crooks and Sooks (0)</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Brooks, Crooks and Sooks</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Kingcalvin (2)</t>
+          <t>Kingcalvin (0)</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Lick DeBallZachs (7)</t>
+          <t>Lick DeBallZachs (0)</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Lick DeBallZachs</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Victor Oladeepthr*ats (3)</t>
+          <t>Victor Oladeepthr*ats (0)</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Who what where when Kawhi (7)</t>
+          <t>Who what where when Kawhi (0)</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Who what where when Kawhi</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>OnlyFranz (4)</t>
+          <t>OnlyFranz (0)</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>The Flaming Galahs (5)</t>
+          <t>The Flaming Galahs (0)</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>The Flaming Galahs</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Dallas Double D's (2)</t>
+          <t>Dallas Double D's (0)</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>G-Town DownTowners (8)</t>
+          <t>G-Town DownTowners (0)</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>G-Town DownTowners</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Memphis 12 Guage (3)</t>
+          <t>Memphis 12 Guage (0)</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Team Alcobio (7)</t>
+          <t>Team Alcobio (0)</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Team Alcobio</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>On The Bagleys (4)</t>
+          <t>On The Bagleys (0)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Wandering Bears (6)</t>
+          <t>Wandering Bears (0)</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Wandering Bears</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Team James (3)</t>
+          <t>Team James (0)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>The A**L Embiids (7)</t>
+          <t>The A**L Embiids (0)</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>The A**L Embiids</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Edward St Easybeats (4)</t>
+          <t>Edward St Easybeats (0)</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>VICTOR-IOUS (6)</t>
+          <t>VICTOR-IOUS (0)</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>VICTOR-IOUS</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Flint Michigan tropics (7)</t>
+          <t>Flint Michigan tropics (0)</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Motor Cade (3)</t>
+          <t>Motor Cade (0)</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Flint Michigan tropics</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Jimmy ButtPlugs (7)</t>
+          <t>Jimmy ButtPlugs (0)</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>The Sengunies (2)</t>
+          <t>The Sengunies (0)</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Jimmy ButtPlugs</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Daryl's Discount Dimes (8)</t>
+          <t>Daryl's Discount Dimes (0)</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Splash Bros 3011 (2)</t>
+          <t>Splash Bros 3011 (0)</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Daryl's Discount Dimes</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Adelaide Shed Shots (7)</t>
+          <t>Adelaide Shed Shots (0)</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Mo' Money Mo Bamba (3)</t>
+          <t>Mo' Money Mo Bamba (0)</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Adelaide Shed Shots</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>ANUS BLEACHING SEA LIONS (5)</t>
+          <t>ANUS BLEACHING SEA LIONS (0)</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>nutted In her Gasol (6)</t>
+          <t>nutted In her Gasol (0)</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>nutted In her Gasol</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Team Cooke (6)</t>
+          <t>Team Cooke (0)</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>The David Cahill's (4)</t>
+          <t>The David Cahill's (0)</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Team Cooke</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Margaret River Wyld Stallyns (6)</t>
+          <t>Margaret River Wyld Stallyns (0)</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Team Damon (5)</t>
+          <t>Team Damon (0)</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Margaret River Wyld Stallyns</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Balls Deep (7)</t>
+          <t>Balls Deep (0)</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Team luka slo (3)</t>
+          <t>Team luka slo (0)</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Balls Deep</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Browntown (3)</t>
+          <t>Browntown (0)</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Seattle SuperChronics (6)</t>
+          <t>Seattle SuperChronics (0)</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Seattle SuperChronics</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Globetrotter Gunts (5)</t>
+          <t>Globetrotter Gunts (0)</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Luka Warm (6)</t>
+          <t>Luka Warm (0)</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Luka Warm</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Bronsexual Lebrolites (3)</t>
+          <t>Bronsexual Lebrolites (0)</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Team Wallace (7)</t>
+          <t>Team Wallace (0)</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Team Wallace</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Atlanta Waivers (4)</t>
+          <t>Atlanta Waivers (0)</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>It's Always F'd In Philadelphia (5)</t>
+          <t>It's Always F'd In Philadelphia (0)</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>It's Always F'd In Philadelphia</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>FIGJAM (4)</t>
+          <t>FIGJAM (0)</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>TankCity Unicorns (6)</t>
+          <t>TankCity Unicorns (0)</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>TankCity Unicorns</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
@@ -1023,735 +1023,735 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Jazz (10)</t>
+          <t>Jazz (0)</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Jazz</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Boswell Pioneers (7)</t>
+          <t>Boswell Pioneers (0)</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>misq (3)</t>
+          <t>misq (0)</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Boswell Pioneers</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Boots Manuva (6)</t>
+          <t>Boots Manuva (0)</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Holy Klay-Noli's (4)</t>
+          <t>Holy Klay-Noli's (0)</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Boots Manuva</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Logan Bogans (7)</t>
+          <t>Logan Bogans (0)</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Minnesota Lumberjacks (3)</t>
+          <t>Minnesota Lumberjacks (0)</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Logan Bogans</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Donnys Beans (6)</t>
+          <t>Donnys Beans (0)</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Livin' La Vida Luka (4)</t>
+          <t>Livin' La Vida Luka (0)</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Donnys Beans</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Good Problems (6)</t>
+          <t>Good Problems (0)</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Rated PG13 (4)</t>
+          <t>Rated PG13 (0)</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Good Problems</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>'22 Spirit (6)</t>
+          <t>'22 Spirit (0)</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>GOLD COAST GREMLINS (4)</t>
+          <t>GOLD COAST GREMLINS (0)</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>'22 Spirit</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Bames Jond (5)</t>
+          <t>Bames Jond (0)</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Diamond D Dynasty (6)</t>
+          <t>Diamond D Dynasty (0)</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Diamond D Dynasty</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>BigZ Spurs (6)</t>
+          <t>BigZ Spurs (0)</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Team irwin (5)</t>
+          <t>Team irwin (0)</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>BigZ Spurs</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Darwin Esky (3)</t>
+          <t>Darwin Esky (0)</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Uncle Ben (7)</t>
+          <t>Uncle Ben (0)</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Uncle Ben</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>MrPenPen (4)</t>
+          <t>MrPenPen (0)</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>The Book of Irving (7)</t>
+          <t>The Book of Irving (0)</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>The Book of Irving</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Scottie Pippings (5)</t>
+          <t>Scottie Pippings (0)</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Zions Illegitimate Child (4)</t>
+          <t>Zions Illegitimate Child (0)</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Scottie Pippings</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Landsdale Smith (6)</t>
+          <t>Landsdale Smith (0)</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>The Hairy Skips (4)</t>
+          <t>The Hairy Skips (0)</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Landsdale Smith</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Round Mound of Rebound (6)</t>
+          <t>Round Mound of Rebound (0)</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Victor WembanYoMama (5)</t>
+          <t>Victor WembanYoMama (0)</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Round Mound of Rebound</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Meep Meep (6)</t>
+          <t>Meep Meep (0)</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Ol' Dirty Baskets (5)</t>
+          <t>Ol' Dirty Baskets (0)</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Meep Meep</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Bulls (6)</t>
+          <t>Bulls (0)</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Team Hewish (5)</t>
+          <t>Team Hewish (0)</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Bulls</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Bank Town Squids (6)</t>
+          <t>Bank Town Squids (0)</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>You Don't Mess with the Ant-Man (4)</t>
+          <t>You Don't Mess with the Ant-Man (0)</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Bank Town Squids</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>The IBINATORS (4)</t>
+          <t>The IBINATORS (0)</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Under my Clint Capela (7)</t>
+          <t>Under my Clint Capela (0)</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Under my Clint Capela</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>ChixnGrog (6)</t>
+          <t>ChixnGrog (0)</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Panania Rockets (4)</t>
+          <t>Panania Rockets (0)</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>ChixnGrog</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>The Bricks (8)</t>
+          <t>The Bricks (0)</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Weekend at Boogie's (2)</t>
+          <t>Weekend at Boogie's (0)</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>The Bricks</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Seattle Superchronics (2)</t>
+          <t>Seattle Superchronics (0)</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>The Gee Whizzles (7)</t>
+          <t>The Gee Whizzles (0)</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>The Gee Whizzles</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Brisbane Noble’s Nobs (4)</t>
+          <t>Brisbane Noble’s Nobs (0)</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Philderbeasts (6)</t>
+          <t>Philderbeasts (0)</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Philderbeasts</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Ja Raffe (7)</t>
+          <t>Ja Raffe (0)</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Team Mercer (3)</t>
+          <t>Team Mercer (0)</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Ja Raffe</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Caruso BaldEagles (6)</t>
+          <t>Caruso BaldEagles (0)</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>I Felton Her Booby (4)</t>
+          <t>I Felton Her Booby (0)</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Caruso BaldEagles</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Big Bam Theory (5)</t>
+          <t>Big Bam Theory (0)</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Triple Towers (6)</t>
+          <t>Triple Towers (0)</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Triple Towers</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Ben Simmons Construction (9)</t>
+          <t>Ben Simmons Construction (0)</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Insert Team Name Here (1)</t>
+          <t>Insert Team Name Here (0)</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Ben Simmons Construction</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Karl Anthony's CLOWNS (5)</t>
+          <t>Karl Anthony's CLOWNS (0)</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Revenge of The Cedi (6)</t>
+          <t>Revenge of The Cedi (0)</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Revenge of The Cedi</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Knock the Toppin off (2)</t>
+          <t>Knock the Toppin off (0)</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Mamba Mentality (8)</t>
+          <t>Mamba Mentality (0)</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Mamba Mentality</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Sleepers (7)</t>
+          <t>Sleepers (0)</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Team Rah to the Max (3)</t>
+          <t>Team Rah to the Max (0)</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Sleepers</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Jackie Daytona (3)</t>
+          <t>Jackie Daytona (0)</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Joeys Mad Lads (7)</t>
+          <t>Joeys Mad Lads (0)</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Joeys Mad Lads</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Kripsy Strips Porzingerbox (5)</t>
+          <t>Kripsy Strips Porzingerbox (0)</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>THE FRESH PRINCE OF GC (6)</t>
+          <t>THE FRESH PRINCE OF GC (0)</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>THE FRESH PRINCE OF GC</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Dort Stop Believin (7)</t>
+          <t>Dort Stop Believin (0)</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Saint Lunatics (3)</t>
+          <t>Saint Lunatics (0)</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Dort Stop Believin</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>HARDEN UP! (4)</t>
+          <t>HARDEN UP! (0)</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Moon Shooters (5)</t>
+          <t>Moon Shooters (0)</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Moon Shooters</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Boston Bombers (4)</t>
+          <t>Boston Bombers (0)</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Don't Go Blakin My Heart (6)</t>
+          <t>Don't Go Blakin My Heart (0)</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Don't Go Blakin My Heart</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Boomtown Bulls (4)</t>
+          <t>Boomtown Bulls (0)</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Shanghai Sharks (6)</t>
+          <t>Shanghai Sharks (0)</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Shanghai Sharks</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Boston Ballerz (3)</t>
+          <t>Boston Ballerz (0)</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Duncans Donuts (7)</t>
+          <t>Duncans Donuts (0)</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Duncans Donuts</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Jaylen CAN go left! (8)</t>
+          <t>Jaylen CAN go left! (0)</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Phoenix Gray Hammers (2)</t>
+          <t>Phoenix Gray Hammers (0)</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Jaylen CAN go left!</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>

</xml_diff>